<commit_message>
Add package information to Telegram base classes.
</commit_message>
<xml_diff>
--- a/meta/objects/ApiDeleteTelegram.xlsx
+++ b/meta/objects/ApiDeleteTelegram.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haino/Desktop/blancoRest/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRest/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>クラス名</t>
   </si>
@@ -136,6 +136,10 @@
   </si>
   <si>
     <t>blanco\rest\valueobject</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>\blanco\sample\valueobject</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -223,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -563,13 +567,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -645,6 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1054,10 +1068,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1202,86 +1216,86 @@
       <c r="J13" s="35"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="42" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B18" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D18" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E18" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F18" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="15"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="30"/>
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
@@ -1293,7 +1307,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
@@ -1313,7 +1327,7 @@
       <c r="B22" s="20"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
-      <c r="E22" s="31"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="21"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
@@ -1385,7 +1399,7 @@
       <c r="B28" s="20"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="21"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
@@ -1429,29 +1443,53 @@
       <c r="J31" s="15"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="28"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="23"/>
       <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F16:G17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E48">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E50">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Correct namespace of telegrams.
</commit_message>
<xml_diff>
--- a/meta/objects/ApiDeleteTelegram.xlsx
+++ b/meta/objects/ApiDeleteTelegram.xlsx
@@ -139,7 +139,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>\blanco\sample\valueobject</t>
+    <t>\blanco\rest\valueobject</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -227,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -567,22 +567,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -658,7 +649,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1071,7 +1061,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1217,23 +1207,23 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="45"/>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="39"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>

</xml_diff>